<commit_message>
updated burn type classified logic, drafted logic for filtering unique burns, drafted leaflet map
</commit_message>
<xml_diff>
--- a/attributexwalk.xlsx
+++ b/attributexwalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5391191E-9FAD-4703-B229-06170850D8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A3417-2273-4947-ACA1-2F01A9177903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attributexwalk" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="200">
   <si>
     <t>AZ</t>
   </si>
@@ -532,42 +532,10 @@
     <t>calc from Burn Number: last digit P is pile, last digit B is broadcast</t>
   </si>
   <si>
-    <r>
-      <t>88370 of 263812 records have the same lat/lon; 10/30 emailed scott philips;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> finish script after scott responds</t>
-    </r>
-  </si>
-  <si>
     <t>Status, no burn reason?</t>
   </si>
   <si>
     <t>calc as [Tons/Acre * acres burned] when Acres Burned was &gt;= 1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">emailed troy w/ questions that are in the script; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>finish when I get response</t>
-    </r>
   </si>
   <si>
     <t>origional spreadsheet had 1 tab per year 2010-2022. I saved each tab as its own file. 
@@ -759,12 +727,15 @@
 -saved 2018, 2021 and 2022 as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
     </r>
   </si>
+  <si>
+    <t>88370 of 263812 records have the same lat/lon; ID can't explain this</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,14 +885,6 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1300,7 +1263,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1362,6 +1325,9 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1740,9 +1706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1817,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -1838,7 +1802,7 @@
         <v>68</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>80</v>
@@ -1879,7 +1843,7 @@
         <v>10</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>76</v>
@@ -1964,7 +1928,7 @@
         <v>147</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>70</v>
@@ -2023,7 +1987,7 @@
         <v>148</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>26</v>
@@ -2107,7 +2071,7 @@
         <v>152</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>31</v>
@@ -2154,7 +2118,7 @@
         <v>150</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>75</v>
@@ -2201,7 +2165,7 @@
         <v>150</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>75</v>
@@ -2224,7 +2188,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J12" s="6"/>
       <c r="L12" s="27" t="s">
@@ -2242,7 +2206,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>151</v>
@@ -2266,10 +2230,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>131</v>
@@ -2284,22 +2248,22 @@
         <v>137</v>
       </c>
       <c r="K14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="N14" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="O14" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -2409,16 +2373,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>120</v>
@@ -2427,10 +2391,10 @@
         <v>121</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2530,7 +2494,7 @@
         <v>118</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>118</v>
@@ -2620,14 +2584,14 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2663,7 +2627,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" s="11"/>
     </row>
@@ -2677,9 +2641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2723,7 +2687,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -2734,7 +2698,7 @@
         <v>126</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>125</v>
@@ -2748,19 +2712,18 @@
         <v>56</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>161</v>
-      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
@@ -2804,10 +2767,10 @@
         <v>145</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
@@ -2818,10 +2781,10 @@
         <v>101</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2832,7 +2795,7 @@
         <v>72</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>95</v>
@@ -2846,10 +2809,10 @@
         <v>99</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -2857,10 +2820,10 @@
         <v>142</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -2868,10 +2831,10 @@
         <v>143</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -2879,10 +2842,10 @@
         <v>144</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated MakeDatabaseSpatialOperations, leaflet map
added routine to get the lifeform and pad info for each point
</commit_message>
<xml_diff>
--- a/attributexwalk.xlsx
+++ b/attributexwalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A3417-2273-4947-ACA1-2F01A9177903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A765134-5E28-4B4A-95C9-B7562FC53B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attributexwalk" sheetId="1" r:id="rId1"/>
@@ -628,6 +628,77 @@
 legal descriptions could be added; I did not include them b/c it looked like lat/lon values were present for every burn</t>
   </si>
   <si>
+    <t>classify all as "Unknown"</t>
+  </si>
+  <si>
+    <t>UT provided spreadsheets for burn permits, requests, and emsissions report. I tried to join them based on the burn name, but this resulted in illogical combinations (e.g. dates on the requests can be in different years than the burn date and the burn date can be before the request date). I couldn't be sure that the right request was going w/ the right emissions report especially for units with multiple entries. Therefore, I used emissions data only for burns that were reported as completed. This probably means we have relatively complete info for completed burns but nothing for burns that were requested but did not occur.
+According to the data provider: "Burn bosses must file an emissions report for each burn request, whether they actually burn or not.  So if a row in the emissions table has "TRUE" under "no_burn", that was not a burn day."  I removed NO burn days b/c it seemed onerous and not super useful to track a bunch or requests that resulted in no burn.</t>
+  </si>
+  <si>
+    <t>classify as complete (no_burn has complete vs. not but I filtered out NO burn days; see processing notes)</t>
+  </si>
+  <si>
+    <t>calc based on Tons</t>
+  </si>
+  <si>
+    <t>calc based on PostBurnArea</t>
+  </si>
+  <si>
+    <t>Burned?</t>
+  </si>
+  <si>
+    <t>origional had columns A-AB, in excel I added:
+BURNTYPE field added and populated: if the daily acres or volume fields specified that piles were burned, I specified the BURNTYPE as Pile
+DAYxMAXACRES = DBI Day X Maximum Area Possible (Acres) but removed alpha characters
+DAYxMAXVOL = DBI Day X Maximum Pile Volume Possible (cubic feet) but removed alpha characters
+PERMITTED_ACRES = sum of all the DAYxMAXACRES fields
+PILE_VOLUME = sum of all the DAYxMAXVOL fields
+removed one illogical date from Daily Burn Information (DBI) Day 1 Date
+-saved as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
+  </si>
+  <si>
+    <t>origional had columns A-P, in excell I added:
+LAT_PERMIT/LON_PERMIT = Latitude/longitude w/o alpha values
+removed extra period in one Lat
+-saved as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
+  </si>
+  <si>
+    <t>extract more info about burn type for BURNTYPE_CLASSIFIED field from burn names
+lat/lon corrections</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I made the following modification in excel:
+2021: deleted "Agency ID" tab
+2018: Saved the "AgencyIDTable" tab as a unique csv to join the AgencyGroup info
+2013: saved "Township Locations" tab as a unique csv to join the Legal descriptions when no lat/lon
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2010: deleted the 2010 tab per Christina's instruction; relevant data are on remaining tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-saved 2018, 2021 and 2022 as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
+    </r>
+  </si>
+  <si>
+    <t>88370 of 263812 records have the same lat/lon; ID can't explain this</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -658,77 +729,6 @@
       </rPr>
       <t xml:space="preserve"> in excel for every tab I did: select all data, clear formats, remove header rows, save as csv</t>
     </r>
-  </si>
-  <si>
-    <t>classify all as "Unknown"</t>
-  </si>
-  <si>
-    <t>UT provided spreadsheets for burn permits, requests, and emsissions report. I tried to join them based on the burn name, but this resulted in illogical combinations (e.g. dates on the requests can be in different years than the burn date and the burn date can be before the request date). I couldn't be sure that the right request was going w/ the right emissions report especially for units with multiple entries. Therefore, I used emissions data only for burns that were reported as completed. This probably means we have relatively complete info for completed burns but nothing for burns that were requested but did not occur.
-According to the data provider: "Burn bosses must file an emissions report for each burn request, whether they actually burn or not.  So if a row in the emissions table has "TRUE" under "no_burn", that was not a burn day."  I removed NO burn days b/c it seemed onerous and not super useful to track a bunch or requests that resulted in no burn.</t>
-  </si>
-  <si>
-    <t>classify as complete (no_burn has complete vs. not but I filtered out NO burn days; see processing notes)</t>
-  </si>
-  <si>
-    <t>calc based on Tons</t>
-  </si>
-  <si>
-    <t>calc based on PostBurnArea</t>
-  </si>
-  <si>
-    <t>Burned?</t>
-  </si>
-  <si>
-    <t>origional had columns A-AB, in excel I added:
-BURNTYPE field added and populated: if the daily acres or volume fields specified that piles were burned, I specified the BURNTYPE as Pile
-DAYxMAXACRES = DBI Day X Maximum Area Possible (Acres) but removed alpha characters
-DAYxMAXVOL = DBI Day X Maximum Pile Volume Possible (cubic feet) but removed alpha characters
-PERMITTED_ACRES = sum of all the DAYxMAXACRES fields
-PILE_VOLUME = sum of all the DAYxMAXVOL fields
-removed one illogical date from Daily Burn Information (DBI) Day 1 Date
--saved as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
-  </si>
-  <si>
-    <t>origional had columns A-P, in excell I added:
-LAT_PERMIT/LON_PERMIT = Latitude/longitude w/o alpha values
-removed extra period in one Lat
--saved as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
-  </si>
-  <si>
-    <t>extract more info about burn type for BURNTYPE_CLASSIFIED field from burn names
-lat/lon corrections</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">I made the following modification in excel:
-2021: deleted "Agency ID" tab
-2018: Saved the "AgencyIDTable" tab as a unique csv to join the AgencyGroup info
-2013: saved "Township Locations" tab as a unique csv to join the Legal descriptions when no lat/lon
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2010: deleted the 2010 tab per Christina's instruction; relevant data are on remaining tab</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--saved 2018, 2021 and 2022 as csv utf-8 so that special characters in burn name would be read in correctly (if saved as regular csv, special characters displayed as diamond with a quesiton mark)</t>
-    </r>
-  </si>
-  <si>
-    <t>88370 of 263812 records have the same lat/lon; ID can't explain this</t>
   </si>
 </sst>
 </file>
@@ -1706,7 +1706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>158</v>
@@ -2248,22 +2248,22 @@
         <v>137</v>
       </c>
       <c r="K14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="M14" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="N14" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="O14" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -2641,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2698,7 +2698,7 @@
         <v>126</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>125</v>
@@ -2712,7 +2712,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2767,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>187</v>
@@ -2781,7 +2781,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>186</v>
@@ -2812,7 +2812,7 @@
         <v>177</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -2823,7 +2823,7 @@
         <v>175</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -2834,7 +2834,7 @@
         <v>174</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>